<commit_message>
Add profiles, dataset and examples for Zib AbilityToManageMedication
</commit_message>
<xml_diff>
--- a/Mappings/AbilityToManageMedication - STU3.xlsx
+++ b/Mappings/AbilityToManageMedication - STU3.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="153">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t xml:space="preserve">.requiredAssistance.reference,  (with .requiredAssistance as an extension)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We could use .related for this, but according to the spec ‘Observation.related is used for any supporting result that can be interpreted and used on its own [...]’. This is not the case for our current situation.</t>
   </si>
   <si>
     <t xml:space="preserve">Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.4.35.1</t>
@@ -829,9 +832,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1797840</xdr:colOff>
+      <xdr:colOff>1797480</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -845,7 +848,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="611280" y="4572000"/>
-          <a:ext cx="2856600" cy="618120"/>
+          <a:ext cx="2856240" cy="617760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -866,9 +869,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6508080</xdr:colOff>
+      <xdr:colOff>6507720</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>249840</xdr:rowOff>
+      <xdr:rowOff>249480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -882,7 +885,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6750000" y="4825800"/>
-          <a:ext cx="1428120" cy="504000"/>
+          <a:ext cx="1427760" cy="503640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,9 +911,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>282600</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -924,7 +927,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="634320" y="635040"/>
-          <a:ext cx="6374520" cy="3761640"/>
+          <a:ext cx="6374160" cy="3761280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,7 +949,7 @@
   </sheetPr>
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1076,7 +1079,7 @@
   </sheetPr>
   <dimension ref="B2:C25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1293,7 +1296,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1324,7 +1327,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1333,7 +1336,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="60.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
@@ -1529,8 +1532,8 @@
   </sheetPr>
   <dimension ref="B2:T5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O14" activeCellId="0" sqref="O14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1546,7 +1549,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="17" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="34.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1679,7 +1683,7 @@
       </c>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
         <v>122</v>
@@ -1716,7 +1720,9 @@
         <v>121</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="T5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1740,7 +1746,7 @@
   </sheetPr>
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1761,23 +1767,23 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>1</v>
@@ -1785,53 +1791,53 @@
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1862,7 @@
   </sheetPr>
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1869,32 +1875,32 @@
   <sheetData>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>